<commit_message>
Added more temperature data points
</commit_message>
<xml_diff>
--- a/Temp calibration.xlsx
+++ b/Temp calibration.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/magnus/Developer/lelit-bianca-protocol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9B07E1-9F83-F346-8825-FA4CEE4A4C31}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8533A467-0AFE-514D-9742-7590C9F90516}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3520" yWindow="460" windowWidth="28040" windowHeight="17440" xr2:uid="{78911000-10DE-494A-9DDF-F5B21CFF0B38}"/>
+    <workbookView xWindow="2160" yWindow="1520" windowWidth="28040" windowHeight="17440" xr2:uid="{78911000-10DE-494A-9DDF-F5B21CFF0B38}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,6 +31,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -221,7 +243,8 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -231,32 +254,6 @@
                   <c:y val="-1.5410964367514842E-2"/>
                 </c:manualLayout>
               </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="65000"/>
-                            <a:lumOff val="35000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:defRPr>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1600" baseline="0"/>
-                      <a:t>y = -0.1342x + 119.71</a:t>
-                    </a:r>
-                    <a:endParaRPr lang="en-US" sz="1600"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -289,132 +286,726 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$30</c:f>
+              <c:f>Sheet1!$A$2:$A$140</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="139"/>
                 <c:pt idx="0">
-                  <c:v>141</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>167</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>164</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>163</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>747</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>661</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>625</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>621</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>612</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>682</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>665</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>654</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>44</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>181</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>220</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>38</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>163</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>202</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>214</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>229</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>233</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>249</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>261</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>272</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>273</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>278</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>282</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>283</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>311</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>316</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>321</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>322</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>327</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>341</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>343</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>347</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>352</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>353</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>355</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>359</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>392</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>394</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>395</c:v>
+                </c:pt>
+                <c:pt idx="77">
                   <c:v>396</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="78">
+                  <c:v>411</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>612</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>621</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>625</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>649</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>654</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>661</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>665</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>682</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>686</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>687</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>696</c:v>
+                </c:pt>
+                <c:pt idx="90">
                   <c:v>697</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>712</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>713</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>714</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>715</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>747</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>743</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>736</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>733</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>729</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>719</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>713</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>644</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>637</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>631</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>607</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>596</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>571</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>559</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>542</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>521</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>508</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>488</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>472</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>452</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>422</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$30</c:f>
+              <c:f>Sheet1!$B$2:$B$140</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="139"/>
                 <c:pt idx="0">
-                  <c:v>99</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>94</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>95</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>95</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>37</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>37</c:v>
+                  <c:v>119</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>38</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>29</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>32</c:v>
+                  <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>33</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>121</c:v>
+                  <c:v>114</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>92</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>86</c:v>
+                  <c:v>111</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>122</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="74">
                   <c:v>64</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="75">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="89">
                   <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>61</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -693,7 +1284,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
+              <c:f>Sheet1!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -734,7 +1325,8 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -744,32 +1336,6 @@
                   <c:y val="4.69095925053164E-2"/>
                 </c:manualLayout>
               </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="65000"/>
-                            <a:lumOff val="35000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:defRPr>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1600" baseline="0"/>
-                      <a:t>y = -0.1402x + 131.65</a:t>
-                    </a:r>
-                    <a:endParaRPr lang="en-US" sz="1600"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -802,96 +1368,192 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$31</c:f>
+              <c:f>Sheet1!$G$2:$G$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
-                  <c:v>104</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>62</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>59</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>114</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>184</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>387</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>617</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>684</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>387</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>184</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>119</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>617</c:v>
+                <c:pt idx="13">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>295</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>296</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>476</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>406</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>405</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>362</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>357</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>337</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>335</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>333</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>729</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>705</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>689</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$31</c:f>
+              <c:f>Sheet1!$H$2:$H$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="44"/>
                 <c:pt idx="0">
-                  <c:v>116</c:v>
+                  <c:v>127</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>127</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>114</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>37</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>126</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>74</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>102</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>113</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>125</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>48</c:v>
+                <c:pt idx="13">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2206,16 +2868,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>387350</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>120650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2242,16 +2904,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>450850</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>196850</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2576,264 +3238,1157 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F526344A-E92A-4F4F-8163-E1515C661948}">
-  <dimension ref="A1:Q38"/>
+  <dimension ref="A1:T119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>141</v>
+        <v>38</v>
       </c>
       <c r="B2">
-        <v>99</v>
-      </c>
-      <c r="D2">
+        <v>122</v>
+      </c>
+      <c r="G2">
+        <v>59</v>
+      </c>
+      <c r="H2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>41</v>
+      </c>
+      <c r="B3">
+        <v>122</v>
+      </c>
+      <c r="G3">
+        <v>61</v>
+      </c>
+      <c r="H3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>43</v>
+      </c>
+      <c r="B4">
+        <v>121</v>
+      </c>
+      <c r="D4" t="e" cm="1">
+        <f t="array" ref="D4">LIN</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G4">
+        <v>62</v>
+      </c>
+      <c r="H4">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>44</v>
+      </c>
+      <c r="B5">
+        <v>121</v>
+      </c>
+      <c r="G5">
+        <v>64</v>
+      </c>
+      <c r="H5">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>44</v>
+      </c>
+      <c r="B6">
+        <v>121</v>
+      </c>
+      <c r="G6">
+        <v>95</v>
+      </c>
+      <c r="H6">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>45</v>
+      </c>
+      <c r="B7">
+        <v>120</v>
+      </c>
+      <c r="G7">
         <v>104</v>
       </c>
-      <c r="E2">
+      <c r="H7">
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>167</v>
-      </c>
-      <c r="B3">
-        <v>94</v>
-      </c>
-      <c r="D3">
-        <v>62</v>
-      </c>
-      <c r="E3">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>164</v>
-      </c>
-      <c r="B4">
-        <v>95</v>
-      </c>
-      <c r="D4">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>48</v>
+      </c>
+      <c r="B8">
+        <v>119</v>
+      </c>
+      <c r="G8">
+        <v>114</v>
+      </c>
+      <c r="H8">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>50</v>
+      </c>
+      <c r="B9">
+        <v>119</v>
+      </c>
+      <c r="G9">
+        <v>119</v>
+      </c>
+      <c r="H9">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>51</v>
+      </c>
+      <c r="B10">
+        <v>118</v>
+      </c>
+      <c r="G10">
+        <v>184</v>
+      </c>
+      <c r="H10">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>59</v>
       </c>
-      <c r="E4">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>163</v>
-      </c>
-      <c r="B5">
-        <v>95</v>
-      </c>
-      <c r="D5">
+      <c r="B11">
+        <v>117</v>
+      </c>
+      <c r="G11">
+        <v>200</v>
+      </c>
+      <c r="H11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>61</v>
+      </c>
+      <c r="B12">
+        <v>116</v>
+      </c>
+      <c r="G12">
+        <v>387</v>
+      </c>
+      <c r="H12">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>63</v>
+      </c>
+      <c r="B13">
+        <v>115</v>
+      </c>
+      <c r="G13">
+        <v>617</v>
+      </c>
+      <c r="H13">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>67</v>
+      </c>
+      <c r="B14">
         <v>114</v>
       </c>
-      <c r="E5">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>747</v>
-      </c>
-      <c r="B6">
-        <v>18</v>
-      </c>
-      <c r="D6">
-        <v>95</v>
-      </c>
-      <c r="E6">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>661</v>
-      </c>
-      <c r="B7">
-        <v>32</v>
-      </c>
-      <c r="D7">
+      <c r="G14">
         <v>684</v>
       </c>
-      <c r="E7">
+      <c r="H14">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>625</v>
-      </c>
-      <c r="B8">
-        <v>37</v>
-      </c>
-      <c r="D8">
-        <v>61</v>
-      </c>
-      <c r="E8">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>621</v>
-      </c>
-      <c r="B9">
-        <v>37</v>
-      </c>
-      <c r="D9">
-        <v>200</v>
-      </c>
-      <c r="E9">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>612</v>
-      </c>
-      <c r="B10">
-        <v>38</v>
-      </c>
-      <c r="D10">
-        <v>387</v>
-      </c>
-      <c r="E10">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>682</v>
-      </c>
-      <c r="B11">
-        <v>29</v>
-      </c>
-      <c r="D11">
-        <v>184</v>
-      </c>
-      <c r="E11">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>665</v>
-      </c>
-      <c r="B12">
-        <v>32</v>
-      </c>
-      <c r="D12">
-        <v>119</v>
-      </c>
-      <c r="E12">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>654</v>
-      </c>
-      <c r="B13">
-        <v>33</v>
-      </c>
-      <c r="D13">
-        <v>64</v>
-      </c>
-      <c r="E13">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>44</v>
-      </c>
-      <c r="B14">
-        <v>121</v>
-      </c>
-      <c r="D14">
-        <v>617</v>
-      </c>
-      <c r="E14">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>181</v>
+        <v>79</v>
       </c>
       <c r="B15">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+      <c r="G15">
+        <v>173</v>
+      </c>
+      <c r="H15">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>220</v>
+        <v>82</v>
       </c>
       <c r="B16">
+        <v>111</v>
+      </c>
+      <c r="G16">
+        <v>295</v>
+      </c>
+      <c r="H16">
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>38</v>
+        <v>84</v>
       </c>
       <c r="B17">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+      <c r="G17">
+        <v>296</v>
+      </c>
+      <c r="H17">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>106</v>
       </c>
       <c r="B18">
         <v>106</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <v>510</v>
+      </c>
+      <c r="H18">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
+        <v>107</v>
+      </c>
+      <c r="B19">
+        <v>106</v>
+      </c>
+      <c r="G19">
+        <v>476</v>
+      </c>
+      <c r="H19">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>108</v>
+      </c>
+      <c r="B20">
+        <v>105</v>
+      </c>
+      <c r="G20">
+        <v>406</v>
+      </c>
+      <c r="H20">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>112</v>
+      </c>
+      <c r="B21">
+        <v>104</v>
+      </c>
+      <c r="G21">
+        <v>405</v>
+      </c>
+      <c r="H21">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>114</v>
+      </c>
+      <c r="B22">
+        <v>104</v>
+      </c>
+      <c r="G22">
+        <v>365</v>
+      </c>
+      <c r="H22">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>116</v>
+      </c>
+      <c r="B23">
+        <v>103</v>
+      </c>
+      <c r="G23">
+        <v>362</v>
+      </c>
+      <c r="H23">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>126</v>
+      </c>
+      <c r="B24">
+        <v>102</v>
+      </c>
+      <c r="G24">
+        <v>357</v>
+      </c>
+      <c r="H24">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>132</v>
+      </c>
+      <c r="B25">
+        <v>101</v>
+      </c>
+      <c r="G25">
+        <v>337</v>
+      </c>
+      <c r="H25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>141</v>
+      </c>
+      <c r="B26">
+        <v>99</v>
+      </c>
+      <c r="G26">
+        <v>335</v>
+      </c>
+      <c r="H26">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>142</v>
+      </c>
+      <c r="B27">
+        <v>99</v>
+      </c>
+      <c r="G27">
+        <v>333</v>
+      </c>
+      <c r="H27">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>143</v>
+      </c>
+      <c r="B28">
+        <v>98</v>
+      </c>
+      <c r="G28">
+        <v>729</v>
+      </c>
+      <c r="H28">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>147</v>
+      </c>
+      <c r="B29">
+        <v>98</v>
+      </c>
+      <c r="G29">
+        <v>705</v>
+      </c>
+      <c r="H29">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>149</v>
+      </c>
+      <c r="B30">
+        <v>97</v>
+      </c>
+      <c r="G30">
+        <v>689</v>
+      </c>
+      <c r="H30">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>163</v>
+      </c>
+      <c r="B31">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>164</v>
+      </c>
+      <c r="B32">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>167</v>
+      </c>
+      <c r="B33">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>174</v>
+      </c>
+      <c r="B34">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>181</v>
+      </c>
+      <c r="B35">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>186</v>
+      </c>
+      <c r="B36">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>189</v>
+      </c>
+      <c r="B37">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>192</v>
+      </c>
+      <c r="B38">
+        <v>91</v>
+      </c>
+      <c r="T38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>194</v>
+      </c>
+      <c r="B39">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>202</v>
+      </c>
+      <c r="B40">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>205</v>
+      </c>
+      <c r="B41">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>208</v>
+      </c>
+      <c r="B42">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>210</v>
+      </c>
+      <c r="B43">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>214</v>
+      </c>
+      <c r="B44">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>217</v>
+      </c>
+      <c r="B45">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>220</v>
+      </c>
+      <c r="B46">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>220</v>
+      </c>
+      <c r="B47">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>225</v>
+      </c>
+      <c r="B48">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>228</v>
+      </c>
+      <c r="B49">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>229</v>
+      </c>
+      <c r="B50">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>233</v>
+      </c>
+      <c r="B51">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>240</v>
+      </c>
+      <c r="B52">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>249</v>
+      </c>
+      <c r="B53">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>260</v>
+      </c>
+      <c r="B54">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>261</v>
+      </c>
+      <c r="B55">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>272</v>
+      </c>
+      <c r="B56">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>273</v>
+      </c>
+      <c r="B57">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>275</v>
+      </c>
+      <c r="B58">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>278</v>
+      </c>
+      <c r="B59">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>282</v>
+      </c>
+      <c r="B60">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>283</v>
+      </c>
+      <c r="B61">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>311</v>
+      </c>
+      <c r="B62">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>312</v>
+      </c>
+      <c r="B63">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>312</v>
+      </c>
+      <c r="B64">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>316</v>
+      </c>
+      <c r="B65">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>321</v>
+      </c>
+      <c r="B66">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>322</v>
+      </c>
+      <c r="B67">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>327</v>
+      </c>
+      <c r="B68">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>341</v>
+      </c>
+      <c r="B69">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>343</v>
+      </c>
+      <c r="B70">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>347</v>
+      </c>
+      <c r="B71">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>352</v>
+      </c>
+      <c r="B72">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>353</v>
+      </c>
+      <c r="B73">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>355</v>
+      </c>
+      <c r="B74">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>359</v>
+      </c>
+      <c r="B75">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>392</v>
+      </c>
+      <c r="B76">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>394</v>
+      </c>
+      <c r="B77">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>395</v>
+      </c>
+      <c r="B78">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79">
         <v>396</v>
       </c>
-      <c r="B19">
+      <c r="B79">
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>411</v>
+      </c>
+      <c r="B80">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>612</v>
+      </c>
+      <c r="B81">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>621</v>
+      </c>
+      <c r="B82">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>625</v>
+      </c>
+      <c r="B83">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>649</v>
+      </c>
+      <c r="B84">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>654</v>
+      </c>
+      <c r="B85">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>661</v>
+      </c>
+      <c r="B86">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>665</v>
+      </c>
+      <c r="B87">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>682</v>
+      </c>
+      <c r="B88">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>686</v>
+      </c>
+      <c r="B89">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>687</v>
+      </c>
+      <c r="B90">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>696</v>
+      </c>
+      <c r="B91">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92">
         <v>697</v>
       </c>
-      <c r="B20">
+      <c r="B92">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="17:17" x14ac:dyDescent="0.2">
-      <c r="Q38" t="s">
-        <v>3</v>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>712</v>
+      </c>
+      <c r="B93">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>713</v>
+      </c>
+      <c r="B94">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>714</v>
+      </c>
+      <c r="B95">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>715</v>
+      </c>
+      <c r="B96">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>747</v>
+      </c>
+      <c r="B97">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>743</v>
+      </c>
+      <c r="B98">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>736</v>
+      </c>
+      <c r="B99">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>733</v>
+      </c>
+      <c r="B100">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>729</v>
+      </c>
+      <c r="B101">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>719</v>
+      </c>
+      <c r="B102">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>713</v>
+      </c>
+      <c r="B103">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>700</v>
+      </c>
+      <c r="B104">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>644</v>
+      </c>
+      <c r="B105">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>637</v>
+      </c>
+      <c r="B106">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>631</v>
+      </c>
+      <c r="B107">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>607</v>
+      </c>
+      <c r="B108">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>596</v>
+      </c>
+      <c r="B109">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>571</v>
+      </c>
+      <c r="B110">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>559</v>
+      </c>
+      <c r="B111">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>542</v>
+      </c>
+      <c r="B112">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>521</v>
+      </c>
+      <c r="B113">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>508</v>
+      </c>
+      <c r="B114">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>488</v>
+      </c>
+      <c r="B115">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>472</v>
+      </c>
+      <c r="B116">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>452</v>
+      </c>
+      <c r="B117">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>436</v>
+      </c>
+      <c r="B118">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>422</v>
+      </c>
+      <c r="B119">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B97">
+    <sortCondition ref="A2:A97"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>